<commit_message>
Fix duplicate name issue and update gender identification - Standardize 'Solum Ole Peder Uthus' to 'Ole Peder Uthus Solum' - Add 'bjarne' to male names list - Consolidate duplicate entries for same person - Update all swimming event data with corrected names and gender identification - Regenerate website with fixes
</commit_message>
<xml_diff>
--- a/EndResult/100m Bryst.xlsx
+++ b/EndResult/100m Bryst.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Male_25m" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Male_50m" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Female_25m" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Female_50m" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Male_25m" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Male_50m" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Female_25m" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Female_50m" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>